<commit_message>
editted excel report api
</commit_message>
<xml_diff>
--- a/app/report/report.xlsx
+++ b/app/report/report.xlsx
@@ -651,18 +651,18 @@
       <c r="C9" s="33" t="n"/>
       <c r="D9" s="37" t="inlineStr">
         <is>
-          <t>another</t>
+          <t>string1</t>
         </is>
       </c>
       <c r="E9" s="38" t="n">
         <v>234</v>
       </c>
       <c r="F9" s="38" t="n">
-        <v>123456</v>
+        <v>456</v>
       </c>
       <c r="G9" s="39" t="n"/>
       <c r="H9" s="38" t="n">
-        <v>28888704</v>
+        <v>106704</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="22">
@@ -835,7 +835,7 @@
     </row>
     <row r="31">
       <c r="H31" t="n">
-        <v>28888704</v>
+        <v>106704</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="H32" t="n">
-        <v>28599816.96</v>
+        <v>105636.96</v>
       </c>
     </row>
     <row r="33">
@@ -855,7 +855,7 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>32031794.9952</v>
+        <v>118313.3952</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added hospital pay reservation
</commit_message>
<xml_diff>
--- a/app/report/report.xlsx
+++ b/app/report/report.xlsx
@@ -543,7 +543,7 @@
         </is>
       </c>
       <c r="E2" s="23" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" s="20">
@@ -577,7 +577,7 @@
       </c>
       <c r="E6" s="26" t="inlineStr">
         <is>
-          <t>qaws</t>
+          <t>string</t>
         </is>
       </c>
       <c r="F6" s="27" t="n"/>
@@ -637,20 +637,20 @@
       </c>
       <c r="D9" s="35" t="inlineStr">
         <is>
-          <t>string1</t>
+          <t>string</t>
         </is>
       </c>
       <c r="E9" s="36" t="n">
-        <v>234</v>
+        <v>10</v>
       </c>
       <c r="F9" s="36" t="n">
-        <v>1234</v>
+        <v>2320</v>
       </c>
       <c r="G9" s="37" t="n">
-        <v>1</v>
+        <v>2340</v>
       </c>
       <c r="H9" s="36" t="n">
-        <v>288756</v>
+        <v>23200</v>
       </c>
     </row>
     <row r="10" ht="15" customHeight="1" s="20">
@@ -865,17 +865,17 @@
     </row>
     <row r="31">
       <c r="H31" t="n">
-        <v>106704</v>
+        <v>23200</v>
       </c>
     </row>
     <row r="32">
       <c r="G32" t="inlineStr">
         <is>
-          <t>5.0% скидка билан</t>
+          <t>0.0% скидка билан</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>105636.96</v>
+        <v>23200</v>
       </c>
     </row>
     <row r="33">
@@ -885,7 +885,7 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>118313.3952</v>
+        <v>25984</v>
       </c>
     </row>
   </sheetData>

</xml_diff>